<commit_message>
add notional PDR propulsion system variables
</commit_message>
<xml_diff>
--- a/physics/propulsion/Propulsion System Configs/IMPORT/Motor Data Condensed.xlsx
+++ b/physics/propulsion/Propulsion System Configs/IMPORT/Motor Data Condensed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamt\OneDrive\Organized\Engineering\Academics\NCSU\Fall 2025\MAE 480 Aerospace Vehicle Design\MDAO\physics\propulsion\Propulsion System Configs\IMPORT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F9FBE2-6F5D-4DD8-BA9E-545EB9F4BEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD4D55F-4D10-4D03-B4E1-4710E40CB48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Company</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>Outer Diameter (mm)</t>
+  </si>
+  <si>
+    <t>A60-5XS V4 28-Pole kv420</t>
+  </si>
+  <si>
+    <t>https://hackermotors.us/product/a60-5xs-v4-28-pole-kv420/</t>
   </si>
 </sst>
 </file>
@@ -230,7 +236,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -366,12 +372,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF434343"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF434343"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF434343"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF434343"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF434343"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF434343"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -405,10 +437,19 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -631,7 +672,7 @@
   <dimension ref="A1:R949"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -876,7 +917,7 @@
         <v>49.7</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>23</v>
       </c>
@@ -932,11 +973,59 @@
         <v>49.7</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G6" s="30"/>
-      <c r="N6" s="31"/>
-    </row>
-    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="40">
+        <v>420</v>
+      </c>
+      <c r="D6" s="40">
+        <v>6</v>
+      </c>
+      <c r="E6" s="40">
+        <v>22.2</v>
+      </c>
+      <c r="F6" s="40">
+        <v>9324</v>
+      </c>
+      <c r="G6" s="41">
+        <v>7925.4</v>
+      </c>
+      <c r="H6" s="40">
+        <v>2200</v>
+      </c>
+      <c r="I6" s="42">
+        <v>99.099099100000004</v>
+      </c>
+      <c r="J6" s="40">
+        <v>2.4</v>
+      </c>
+      <c r="K6" s="40">
+        <v>1.2E-2</v>
+      </c>
+      <c r="L6" s="40">
+        <v>480</v>
+      </c>
+      <c r="M6" s="43">
+        <v>297</v>
+      </c>
+      <c r="N6" s="44"/>
+      <c r="O6" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="45">
+        <v>52</v>
+      </c>
+      <c r="R6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="G7" s="30"/>
       <c r="N7" s="31"/>
     </row>
@@ -4715,6 +4804,7 @@
     <hyperlink ref="P3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="O4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="O5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="O6" r:id="rId6" xr:uid="{E5B2A9EB-5F5E-416F-9C24-2951065741A4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
running PDR design all the way through M3 propulsion analysis
</commit_message>
<xml_diff>
--- a/physics/propulsion/Propulsion System Configs/IMPORT/Motor Data Condensed.xlsx
+++ b/physics/propulsion/Propulsion System Configs/IMPORT/Motor Data Condensed.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\liamt\OneDrive\Organized\Engineering\Academics\NCSU\Fall 2025\MAE 480 Aerospace Vehicle Design\MDAO\physics\propulsion\Propulsion System Configs\IMPORT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD4D55F-4D10-4D03-B4E1-4710E40CB48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E826FD4F-D1B8-4E37-80BA-5779C231A738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -403,7 +403,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -441,14 +441,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -672,7 +665,7 @@
   <dimension ref="A1:R949"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -977,48 +970,46 @@
       <c r="A6" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="12">
         <v>420</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="12">
         <v>6</v>
       </c>
-      <c r="E6" s="40">
+      <c r="E6" s="12">
         <v>22.2</v>
       </c>
-      <c r="F6" s="40">
+      <c r="F6" s="12">
         <v>9324</v>
       </c>
-      <c r="G6" s="41">
+      <c r="G6" s="13">
         <v>7925.4</v>
       </c>
-      <c r="H6" s="40">
+      <c r="H6" s="12">
         <v>2200</v>
       </c>
-      <c r="I6" s="42">
+      <c r="I6" s="14">
         <v>99.099099100000004</v>
       </c>
-      <c r="J6" s="40">
+      <c r="K6" s="12">
         <v>2.4</v>
       </c>
-      <c r="K6" s="40">
+      <c r="L6" s="12">
         <v>1.2E-2</v>
       </c>
-      <c r="L6" s="40">
+      <c r="M6" s="12">
         <v>480</v>
       </c>
-      <c r="M6" s="43">
+      <c r="N6" s="15">
         <v>297</v>
       </c>
-      <c r="N6" s="44"/>
-      <c r="O6" s="44" t="s">
+      <c r="O6" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="P6" s="38"/>
-      <c r="Q6" s="45">
+      <c r="Q6" s="38">
         <v>52</v>
       </c>
       <c r="R6">

</xml_diff>